<commit_message>
separate blood and mfp
</commit_message>
<xml_diff>
--- a/tables/de.table.xlsx
+++ b/tables/de.table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ataka\Documents\rewiring\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7F41E0-7828-4D35-A4F3-F7BAC4BAD2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897635C7-0C3C-4CE5-86CF-EE34EEA58923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="12" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="d.AL.49.50.Blood" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,17 @@
     <sheet name="d.CCR.81.82.MFP" sheetId="17" r:id="rId17"/>
     <sheet name="d.ICR.81.82.MFP" sheetId="18" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1158,6 +1168,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1739,7 +1752,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2256,9 +2271,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2454,7 +2474,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2839,9 +2861,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -3086,6 +3113,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -3169,6 +3199,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -3459,6 +3492,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -4183,9 +4219,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -4956,7 +4997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>